<commit_message>
EPBDS-9080 bug fix. Specifying the same parameter in the several columns should be forbidden
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DuplicateIdentifierInTests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DuplicateIdentifierInTests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvlad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F6032-7AFE-4FF1-86EE-DC07E348453C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA89F583-875B-45FF-B49C-C294307412C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Double</t>
   </si>
@@ -104,6 +104,36 @@
       </rPr>
       <t>AnnualPremium</t>
     </r>
+  </si>
+  <si>
+    <t>Test doAnnualPremium duplicatedFieldInDatatype2_negativeTest</t>
+  </si>
+  <si>
+    <t>_res_.rate(1)</t>
+  </si>
+  <si>
+    <t>_res_.rate</t>
+  </si>
+  <si>
+    <t>Test doAnnualPremiumSpr duplicatedFieldInSpr2_negativeTest</t>
+  </si>
+  <si>
+    <t>_res_.$MonthYear</t>
+  </si>
+  <si>
+    <t>_res_.$MonthYear(-2)</t>
+  </si>
+  <si>
+    <t>Test doAnnualPremiumSpr duplicatedFieldInSpr3_negativeTest</t>
+  </si>
+  <si>
+    <t>_res_.$MonthlyPremium(-1)</t>
+  </si>
+  <si>
+    <t>_res_.$MonthlyPremium(-2)</t>
+  </si>
+  <si>
+    <t>_res_.$MonthlyPremium</t>
   </si>
 </sst>
 </file>
@@ -176,18 +206,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:G28"/>
+  <dimension ref="B3:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,213 +521,414 @@
         <v>21</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>0.05</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>5000</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>250</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>240</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>0.05</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>5000</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>250</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>240</v>
       </c>
     </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C38" s="8">
+        <v>5000</v>
+      </c>
+      <c r="D38" s="7">
+        <v>250</v>
+      </c>
+      <c r="E38" s="7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C46" s="8">
+        <v>5000</v>
+      </c>
+      <c r="D46" s="7">
+        <v>250</v>
+      </c>
+      <c r="E46" s="7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C54" s="8">
+        <v>5000</v>
+      </c>
+      <c r="D54" s="7">
+        <v>250</v>
+      </c>
+      <c r="E54" s="7">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B51:E51"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B17:E17"/>

</xml_diff>